<commit_message>
Se actualiza la llamada a los datos de prueba del proyecto. Invocación via DataDriven
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Downloads\DemoFrameworkBootCamp\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71137B1-B1E1-453E-91E6-00ED9CCB8D47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E363A206-CD75-40F6-85A3-5A30E7C27F3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{E6394DFB-6163-4A1C-B561-81F0B75BD956}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -132,9 +132,6 @@
     <t>weqw</t>
   </si>
   <si>
-    <t>qwe</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -205,6 +202,21 @@
   </si>
   <si>
     <t>Confirma que no eres un robot.</t>
+  </si>
+  <si>
+    <t>CP002_Registro_Fallido_Password_Corta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Tu contraseña es demasiado corta.</t>
   </si>
 </sst>
 </file>
@@ -593,7 +605,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,7 +614,7 @@
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -642,66 +654,64 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1">
         <v>123454321</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1">
         <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" s="1">
         <v>1990</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -709,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -751,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -778,7 +788,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -817,19 +827,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C9" s="1">
         <v>123123</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1040,51 +1050,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1099,19 +1109,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1124,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1141,28 +1151,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1172,28 +1182,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1203,13 +1213,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1236,7 +1246,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>

</xml_diff>

<commit_message>
Se refactoriza proyecto. Se construye branch para desafio BC11
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Downloads\DemoFrameworkBootCamp\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E363A206-CD75-40F6-85A3-5A30E7C27F3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFB77E0-29F6-4269-8B40-10EFCC6DDECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{E6394DFB-6163-4A1C-B561-81F0B75BD956}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <sheet name="Hoja7" sheetId="8" r:id="rId8"/>
     <sheet name="Hoja8" sheetId="9" r:id="rId9"/>
     <sheet name="Hoja9" sheetId="10" r:id="rId10"/>
+    <sheet name="Hoja11" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -120,33 +121,6 @@
     <t>Dato N</t>
   </si>
   <si>
-    <t>qweqwe</t>
-  </si>
-  <si>
-    <t>qew</t>
-  </si>
-  <si>
-    <t>qweqw</t>
-  </si>
-  <si>
-    <t>weqw</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Recuerda que tu clave de internet tiene entre</t>
-  </si>
-  <si>
-    <t>incorrecta</t>
-  </si>
-  <si>
-    <t>CP008_Login_Fallido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53991509‑6	</t>
-  </si>
-  <si>
     <t>Dato001</t>
   </si>
   <si>
@@ -189,34 +163,10 @@
     <t>TituloCPs</t>
   </si>
   <si>
-    <t>CP001_Registro_Fallido_Captcha_en_blanco</t>
-  </si>
-  <si>
-    <t>domingo.saavedra@tsoftglobal.com</t>
-  </si>
-  <si>
-    <t>Pobre Domingo</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Confirma que no eres un robot.</t>
-  </si>
-  <si>
-    <t>CP002_Registro_Fallido_Password_Corta</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>Junio</t>
-  </si>
-  <si>
-    <t>Tu contraseña es demasiado corta.</t>
   </si>
 </sst>
 </file>
@@ -605,7 +555,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,83 +603,41 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="1">
-        <v>123454321</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="1">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1990</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -738,15 +646,9 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -757,48 +659,24 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -807,15 +685,9 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -826,21 +698,11 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="1">
-        <v>123123</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -849,9 +711,7 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -864,9 +724,7 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -879,9 +737,7 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -894,9 +750,7 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -909,9 +763,7 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -924,9 +776,7 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -939,9 +789,7 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -954,9 +802,7 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -969,9 +815,7 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -984,9 +828,7 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -999,9 +841,7 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1014,17 +854,27 @@
       <c r="K20" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{6C3FABF3-F2E4-49A9-A370-956F07A210A8}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{07009988-FE24-4C53-B9D9-B51230D7B910}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253A64FB-2406-4BC6-A77B-D51C811F66E0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BDE46B-A4A0-419A-9E00-DD65662C58C7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1050,51 +900,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1109,19 +959,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1134,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1151,28 +1001,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1182,28 +1032,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1213,13 +1063,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1246,7 +1096,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>

</xml_diff>

<commit_message>
Fix funcionalidades Actualizacion caso 001 al 012 operativos
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30EE36-AAA6-4937-918E-932DD43A739B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26DC696-2500-4FFC-A2DE-3F64B01F9BCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
   <si>
     <t>CP012</t>
   </si>
@@ -231,12 +231,6 @@
     <t>Lo sentimos</t>
   </si>
   <si>
-    <t>Fabian</t>
-  </si>
-  <si>
-    <t>Yañez</t>
-  </si>
-  <si>
     <t>Aaron Barra</t>
   </si>
   <si>
@@ -261,9 +255,6 @@
     <t>CP009_BusquedaTrenes_SeleccionarTicketMasBarato</t>
   </si>
   <si>
-    <t>21.46 €</t>
-  </si>
-  <si>
     <t>CP010_BusquedaTrenes_ModificarParametrosOfertasTrenHotel</t>
   </si>
   <si>
@@ -289,13 +280,25 @@
   </si>
   <si>
     <t>CP012_BusquedaTrenes_TarjetaSinFondos</t>
+  </si>
+  <si>
+    <t>5100 0100 0000 0114</t>
+  </si>
+  <si>
+    <t>Messi</t>
+  </si>
+  <si>
+    <t>Lia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_-\ [$€-1]_ ;_ * #,##0.00\-\ [$€-1]_ ;_ * &quot;-&quot;??_-\ [$€-1]_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +325,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -383,6 +394,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -666,16 +679,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1"/>
@@ -957,10 +971,10 @@
         <v>958487569</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="K7" s="2">
         <v>17</v>
@@ -981,10 +995,10 @@
         <v>1999</v>
       </c>
       <c r="Q7" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="R7" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="S7">
         <v>25</v>
@@ -993,10 +1007,10 @@
         <v>1992</v>
       </c>
       <c r="U7" t="s">
-        <v>68</v>
-      </c>
-      <c r="V7" s="5">
-        <v>4051885600446620</v>
+        <v>66</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="W7">
         <v>6</v>
@@ -1017,7 +1031,7 @@
         <v>58</v>
       </c>
       <c r="AC7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AD7">
         <v>2715</v>
@@ -1026,7 +1040,7 @@
         <v>79100000</v>
       </c>
       <c r="AF7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AG7" t="s">
         <v>59</v>
@@ -1037,13 +1051,13 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>46</v>
@@ -1058,7 +1072,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -1067,7 +1081,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1079,16 +1093,16 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="B10" s="7">
+        <v>21.66</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1100,20 +1114,22 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1123,25 +1139,25 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H12" s="2">
         <v>1157966485</v>
@@ -1153,10 +1169,10 @@
         <v>1999</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L12" s="5">
-        <v>4051885600446620</v>
+        <v>81</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="M12">
         <v>11</v>
@@ -1170,7 +1186,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>65</v>
@@ -1179,16 +1195,16 @@
         <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H13" s="2">
         <v>1157966485</v>
@@ -1200,16 +1216,16 @@
         <v>1999</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L13" s="5">
-        <v>4051885600446620</v>
+        <v>81</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="M13">
         <v>11</v>
       </c>
       <c r="N13">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O13">
         <v>123</v>

</xml_diff>

<commit_message>
Se actualiza archivo Data.xlsx, complementando con parámetros de entradas de casos de prueba en Hoteles.
Se actualizan rutas de casos de pruebas en archivo properties.properties.

Se actualiza método handle en BaseClass.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26DC696-2500-4FFC-A2DE-3F64B01F9BCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4306BDEC-C84D-43BB-BFEB-45919C1D876E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28365" yWindow="660" windowWidth="27030" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPruebas" sheetId="1" r:id="rId1"/>
@@ -31,31 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
-  <si>
-    <t>CP012</t>
-  </si>
-  <si>
-    <t>CP013</t>
-  </si>
-  <si>
-    <t>CP014</t>
-  </si>
-  <si>
-    <t>CP015</t>
-  </si>
-  <si>
-    <t>CP016</t>
-  </si>
-  <si>
-    <t>CP017</t>
-  </si>
-  <si>
-    <t>CP018</t>
-  </si>
-  <si>
-    <t>CP00N</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="98">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -289,6 +265,66 @@
   </si>
   <si>
     <t>Lia</t>
+  </si>
+  <si>
+    <t>Introduce un número válido</t>
+  </si>
+  <si>
+    <t>Cancun</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Barcia</t>
+  </si>
+  <si>
+    <t>david.barcia@hotmail.com</t>
+  </si>
+  <si>
+    <t>David Barcia</t>
+  </si>
+  <si>
+    <t>CP013_Reserva_de_hotel_Con_Tarjeta_Num_Invalido</t>
+  </si>
+  <si>
+    <t>CP014_Buscar_2_Habitacion_Con_Desayuno</t>
+  </si>
+  <si>
+    <t>Añadir huéspedes y forma de pago</t>
+  </si>
+  <si>
+    <t>santiago de chile</t>
+  </si>
+  <si>
+    <t>CP015_Buscar_Reserva_de_3_Habitaciones</t>
+  </si>
+  <si>
+    <t>Alojamientos en Toronto</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>CP017_Validar_Datos_Data_Erronea</t>
+  </si>
+  <si>
+    <t>Introduce un email válido</t>
+  </si>
+  <si>
+    <t>davidhotmail.com</t>
+  </si>
+  <si>
+    <t>CP016_Validar_Busqueda_De_Hotel_Con_6_Viajeros</t>
+  </si>
+  <si>
+    <t>https://inspirame.rumbo.es</t>
+  </si>
+  <si>
+    <t>Lo sentimos, no se pueden reservar más de 31 noches</t>
+  </si>
+  <si>
+    <t>CP018_Validar_Reserva_Mayor_A_31_Noches</t>
   </si>
 </sst>
 </file>
@@ -298,7 +334,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_-\ [$€-1]_ ;_ * #,##0.00\-\ [$€-1]_ ;_ * &quot;-&quot;??_-\ [$€-1]_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,14 +353,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -382,23 +410,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{EC9F5DBB-B614-455F-B651-888A016EC857}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -677,173 +709,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD1" s="6" t="s">
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -853,18 +888,18 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -874,18 +909,18 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -895,36 +930,36 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>55</v>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H6" s="2">
         <v>958487569</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K6" s="2">
         <v>17</v>
@@ -933,10 +968,10 @@
         <v>1994</v>
       </c>
       <c r="M6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="O6">
         <v>13</v>
@@ -945,36 +980,36 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H7" s="2">
         <v>958487569</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="K7" s="2">
         <v>17</v>
@@ -983,10 +1018,10 @@
         <v>1994</v>
       </c>
       <c r="M7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="O7">
         <v>13</v>
@@ -995,10 +1030,10 @@
         <v>1999</v>
       </c>
       <c r="Q7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="R7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="S7">
         <v>25</v>
@@ -1007,10 +1042,10 @@
         <v>1992</v>
       </c>
       <c r="U7" t="s">
-        <v>66</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>83</v>
+        <v>58</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="W7">
         <v>6</v>
@@ -1021,17 +1056,17 @@
       <c r="Y7">
         <v>642</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7" s="3">
         <v>165786249</v>
       </c>
       <c r="AA7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="AB7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="AC7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="AD7">
         <v>2715</v>
@@ -1040,27 +1075,27 @@
         <v>79100000</v>
       </c>
       <c r="AF7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AG7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH7" s="5">
+        <v>51</v>
+      </c>
+      <c r="AH7" s="3">
         <v>958487569</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1070,18 +1105,18 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1091,18 +1126,18 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="7">
+        <v>65</v>
+      </c>
+      <c r="B10" s="5">
         <v>21.66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1112,24 +1147,24 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1137,27 +1172,27 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H12" s="2">
         <v>1157966485</v>
@@ -1169,10 +1204,10 @@
         <v>1999</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="M12">
         <v>11</v>
@@ -1184,27 +1219,27 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H13" s="2">
         <v>1157966485</v>
@@ -1216,10 +1251,10 @@
         <v>1999</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="M13">
         <v>11</v>
@@ -1231,27 +1266,51 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="9">
+        <v>23495123</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="9">
+        <v>485829</v>
+      </c>
+      <c r="J14" s="7">
+        <v>12</v>
+      </c>
+      <c r="K14" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1261,12 +1320,16 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1276,12 +1339,16 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1291,27 +1358,51 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="7">
+        <v>23495123</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1321,39 +1412,13 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F14" r:id="rId1" xr:uid="{A5F1841C-F53F-4F64-95D3-88CDA79F8A7F}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{6E725485-D63F-476E-A558-EDFB8E92B5A1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1363,7 +1428,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1375,7 +1440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1387,7 +1452,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1399,7 +1464,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1411,7 +1476,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1423,7 +1488,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1435,7 +1500,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1447,7 +1512,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1459,7 +1524,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1471,7 +1536,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1483,7 +1548,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>